<commit_message>
Ch 2, Ch 3
</commit_message>
<xml_diff>
--- a/Chapter 2/Ch02_Back_Savers.xlsx
+++ b/Chapter 2/Ch02_Back_Savers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vafa.saboorideilami/Documents/5509 Summer 2024/Chapter 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED6C201-A092-C041-8A24-970885EFE3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464A462F-C3E2-F647-B087-15DC1DBD1D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -982,7 +982,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="213" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="E7" s="11">
         <f>SUMPRODUCT(C7:D7,UnitsProduced)</f>
-        <v>5</v>
+        <v>4949.9999999025003</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>12</v>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="E8" s="11">
         <f>SUMPRODUCT(C8:D8,UnitsProduced)</f>
-        <v>1.4166666666999999</v>
+        <v>1400</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>12</v>
@@ -1153,14 +1153,14 @@
         <v>16</v>
       </c>
       <c r="C11" s="20">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D11" s="21">
-        <v>1</v>
+        <v>974.99999995125029</v>
       </c>
       <c r="G11" s="22">
         <f>SUMPRODUCT(UnitProfit,UnitsProduced)</f>
-        <v>56</v>
+        <v>55399.999998830011</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>